<commit_message>
fix: Cleaned up minor issues with SearchSets. It looks like all bindings are working now.
</commit_message>
<xml_diff>
--- a/data/Hospital/TimeLiner-MasterList(Dynamic Dates).xlsx
+++ b/data/Hospital/TimeLiner-MasterList(Dynamic Dates).xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="Hospital" sheetId="1" r:id="rId3"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="994" uniqueCount="508">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="994" uniqueCount="514">
   <si>
     <t>Active</t>
   </si>
@@ -651,7 +651,7 @@
     <t>Arch-Ext-Wall-L1</t>
   </si>
   <si>
-    <t>Sets-&gt;Architectural-&gt;Exterior-&gt;Walls</t>
+    <t>Sets-&gt;Architectural-&gt;Exterior-&gt;Walls-&gt;Arch-Ext-Wall-L1</t>
   </si>
   <si>
     <t>3101-2</t>
@@ -660,34 +660,52 @@
     <t>Arch-Ext-Wall-L2</t>
   </si>
   <si>
+    <t>Sets-&gt;Architectural-&gt;Exterior-&gt;Walls-&gt;Arch-Ext-Wall-L2</t>
+  </si>
+  <si>
     <t>3101-3</t>
   </si>
   <si>
     <t>Arch-Ext-Wall-L3</t>
   </si>
   <si>
+    <t>Sets-&gt;Architectural-&gt;Exterior-&gt;Walls-&gt;Arch-Ext-Wall-L3</t>
+  </si>
+  <si>
     <t>3101-4</t>
   </si>
   <si>
     <t>Arch-Ext-Wall-L4</t>
   </si>
   <si>
+    <t>Sets-&gt;Architectural-&gt;Exterior-&gt;Walls-&gt;Arch-Ext-Wall-L4</t>
+  </si>
+  <si>
     <t>3101-5</t>
   </si>
   <si>
     <t>Arch-Ext-Wall-L5</t>
   </si>
   <si>
+    <t>Sets-&gt;Architectural-&gt;Exterior-&gt;Walls-&gt;Arch-Ext-Wall-L5</t>
+  </si>
+  <si>
     <t>3101-6</t>
   </si>
   <si>
     <t>Arch-Ext-Wall-L6</t>
   </si>
   <si>
+    <t>Sets-&gt;Architectural-&gt;Exterior-&gt;Walls-&gt;Arch-Ext-Wall-L6</t>
+  </si>
+  <si>
     <t>3101-7</t>
   </si>
   <si>
     <t>Arch-Ext-Wall-L7</t>
+  </si>
+  <si>
+    <t>Sets-&gt;Architectural-&gt;Exterior-&gt;Walls-&gt;Arch-Ext-Wall-L7</t>
   </si>
   <si>
     <t>3101-8</t>
@@ -1713,11 +1731,11 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <pageSetUpPr/>
   </sheetPr>
@@ -5831,7 +5849,7 @@
       <c r="K64" t="s">
         <v>43</v>
       </c>
-      <c r="L64" t="s">
+      <c r="L64" s="25" t="s">
         <v>207</v>
       </c>
       <c r="O64" s="21" t="s">
@@ -5895,14 +5913,14 @@
       <c r="K65" t="s">
         <v>43</v>
       </c>
-      <c r="L65" t="s">
-        <v>207</v>
+      <c r="L65" s="25" t="s">
+        <v>210</v>
       </c>
       <c r="O65" s="21" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="P65" s="21" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="R65" t="s">
         <v>35</v>
@@ -5932,7 +5950,7 @@
         <v>1.0</v>
       </c>
       <c r="B66" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C66">
         <v>3.0</v>
@@ -5959,14 +5977,14 @@
       <c r="K66" t="s">
         <v>43</v>
       </c>
-      <c r="L66" t="s">
-        <v>207</v>
+      <c r="L66" s="25" t="s">
+        <v>213</v>
       </c>
       <c r="O66" s="21" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="P66" s="21" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="R66" t="s">
         <v>35</v>
@@ -5996,7 +6014,7 @@
         <v>1.0</v>
       </c>
       <c r="B67" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="C67">
         <v>3.0</v>
@@ -6023,14 +6041,14 @@
       <c r="K67" t="s">
         <v>43</v>
       </c>
-      <c r="L67" t="s">
-        <v>207</v>
+      <c r="L67" s="25" t="s">
+        <v>216</v>
       </c>
       <c r="O67" s="21" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="P67" s="21" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="R67" t="s">
         <v>35</v>
@@ -6060,7 +6078,7 @@
         <v>1.0</v>
       </c>
       <c r="B68" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="C68">
         <v>3.0</v>
@@ -6087,14 +6105,14 @@
       <c r="K68" t="s">
         <v>43</v>
       </c>
-      <c r="L68" t="s">
-        <v>207</v>
+      <c r="L68" s="25" t="s">
+        <v>219</v>
       </c>
       <c r="O68" s="21" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="P68" s="21" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="R68" t="s">
         <v>35</v>
@@ -6124,7 +6142,7 @@
         <v>1.0</v>
       </c>
       <c r="B69" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="C69">
         <v>3.0</v>
@@ -6151,14 +6169,14 @@
       <c r="K69" t="s">
         <v>43</v>
       </c>
-      <c r="L69" t="s">
-        <v>207</v>
+      <c r="L69" s="25" t="s">
+        <v>222</v>
       </c>
       <c r="O69" s="21" t="s">
-        <v>218</v>
+        <v>223</v>
       </c>
       <c r="P69" s="21" t="s">
-        <v>218</v>
+        <v>223</v>
       </c>
       <c r="R69" t="s">
         <v>35</v>
@@ -6188,7 +6206,7 @@
         <v>1.0</v>
       </c>
       <c r="B70" t="s">
-        <v>219</v>
+        <v>224</v>
       </c>
       <c r="C70">
         <v>3.0</v>
@@ -6215,14 +6233,14 @@
       <c r="K70" t="s">
         <v>43</v>
       </c>
-      <c r="L70" t="s">
-        <v>207</v>
+      <c r="L70" s="25" t="s">
+        <v>225</v>
       </c>
       <c r="O70" s="21" t="s">
-        <v>220</v>
+        <v>226</v>
       </c>
       <c r="P70" s="21" t="s">
-        <v>220</v>
+        <v>226</v>
       </c>
       <c r="R70" t="s">
         <v>35</v>
@@ -6252,7 +6270,7 @@
         <v>1.0</v>
       </c>
       <c r="B71" t="s">
-        <v>221</v>
+        <v>227</v>
       </c>
       <c r="C71">
         <v>2.0</v>
@@ -6280,13 +6298,13 @@
         <v>43</v>
       </c>
       <c r="L71" t="s">
-        <v>222</v>
+        <v>228</v>
       </c>
       <c r="O71" s="21" t="s">
-        <v>223</v>
+        <v>229</v>
       </c>
       <c r="P71" s="21" t="s">
-        <v>223</v>
+        <v>229</v>
       </c>
       <c r="R71" t="s">
         <v>35</v>
@@ -6316,7 +6334,7 @@
         <v>1.0</v>
       </c>
       <c r="B72" s="29" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
       <c r="C72" s="29">
         <v>2.0</v>
@@ -6335,10 +6353,10 @@
       <c r="M72" s="29"/>
       <c r="N72" s="29"/>
       <c r="O72" s="31" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
       <c r="P72" s="31" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
       <c r="Q72" s="29"/>
       <c r="R72" s="29" t="s">
@@ -6370,7 +6388,7 @@
         <v>1.0</v>
       </c>
       <c r="B73" t="s">
-        <v>226</v>
+        <v>232</v>
       </c>
       <c r="C73">
         <v>3.0</v>
@@ -6398,13 +6416,13 @@
         <v>43</v>
       </c>
       <c r="L73" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
       <c r="O73" s="21" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
       <c r="P73" s="21" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
       <c r="R73" t="s">
         <v>35</v>
@@ -6435,7 +6453,7 @@
         <v>1.0</v>
       </c>
       <c r="B74" t="s">
-        <v>229</v>
+        <v>235</v>
       </c>
       <c r="C74">
         <v>3.0</v>
@@ -6463,13 +6481,13 @@
         <v>43</v>
       </c>
       <c r="L74" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="O74" s="21" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
       <c r="P74" s="21" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
       <c r="R74" t="s">
         <v>35</v>
@@ -6498,7 +6516,7 @@
         <v>1.0</v>
       </c>
       <c r="B75" t="s">
-        <v>232</v>
+        <v>238</v>
       </c>
       <c r="C75">
         <v>3.0</v>
@@ -6526,13 +6544,13 @@
         <v>43</v>
       </c>
       <c r="L75" t="s">
-        <v>233</v>
+        <v>239</v>
       </c>
       <c r="O75" s="21" t="s">
-        <v>234</v>
+        <v>240</v>
       </c>
       <c r="P75" s="21" t="s">
-        <v>234</v>
+        <v>240</v>
       </c>
       <c r="R75" t="s">
         <v>35</v>
@@ -6561,7 +6579,7 @@
         <v>1.0</v>
       </c>
       <c r="B76" t="s">
-        <v>235</v>
+        <v>241</v>
       </c>
       <c r="C76">
         <v>3.0</v>
@@ -6589,13 +6607,13 @@
         <v>43</v>
       </c>
       <c r="L76" t="s">
-        <v>236</v>
+        <v>242</v>
       </c>
       <c r="O76" s="21" t="s">
-        <v>237</v>
+        <v>243</v>
       </c>
       <c r="P76" s="21" t="s">
-        <v>237</v>
+        <v>243</v>
       </c>
       <c r="R76" t="s">
         <v>35</v>
@@ -6624,7 +6642,7 @@
         <v>1.0</v>
       </c>
       <c r="B77" t="s">
-        <v>238</v>
+        <v>244</v>
       </c>
       <c r="C77">
         <v>3.0</v>
@@ -6652,13 +6670,13 @@
         <v>43</v>
       </c>
       <c r="L77" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="O77" s="21" t="s">
-        <v>240</v>
+        <v>246</v>
       </c>
       <c r="P77" s="21" t="s">
-        <v>240</v>
+        <v>246</v>
       </c>
       <c r="R77" t="s">
         <v>35</v>
@@ -6687,7 +6705,7 @@
         <v>1.0</v>
       </c>
       <c r="B78" t="s">
-        <v>241</v>
+        <v>247</v>
       </c>
       <c r="C78">
         <v>3.0</v>
@@ -6715,13 +6733,13 @@
         <v>43</v>
       </c>
       <c r="L78" t="s">
-        <v>242</v>
+        <v>248</v>
       </c>
       <c r="O78" s="21" t="s">
-        <v>243</v>
+        <v>249</v>
       </c>
       <c r="P78" s="21" t="s">
-        <v>243</v>
+        <v>249</v>
       </c>
       <c r="R78" t="s">
         <v>35</v>
@@ -6750,7 +6768,7 @@
         <v>1.0</v>
       </c>
       <c r="B79" s="29" t="s">
-        <v>244</v>
+        <v>250</v>
       </c>
       <c r="C79" s="29">
         <v>2.0</v>
@@ -6771,10 +6789,10 @@
       <c r="M79" s="29"/>
       <c r="N79" s="29"/>
       <c r="O79" s="31" t="s">
-        <v>245</v>
+        <v>251</v>
       </c>
       <c r="P79" s="31" t="s">
-        <v>245</v>
+        <v>251</v>
       </c>
       <c r="Q79" s="29"/>
       <c r="R79" s="29" t="s">
@@ -6806,7 +6824,7 @@
         <v>1.0</v>
       </c>
       <c r="B80" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
       <c r="C80">
         <v>3.0</v>
@@ -6834,13 +6852,13 @@
         <v>43</v>
       </c>
       <c r="L80" t="s">
-        <v>247</v>
+        <v>253</v>
       </c>
       <c r="O80" s="21" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="P80" s="21" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="R80" t="s">
         <v>35</v>
@@ -6869,7 +6887,7 @@
         <v>1.0</v>
       </c>
       <c r="B81" s="29" t="s">
-        <v>249</v>
+        <v>255</v>
       </c>
       <c r="C81" s="29">
         <v>2.0</v>
@@ -6890,10 +6908,10 @@
       <c r="M81" s="29"/>
       <c r="N81" s="29"/>
       <c r="O81" s="31" t="s">
-        <v>250</v>
+        <v>256</v>
       </c>
       <c r="P81" s="31" t="s">
-        <v>250</v>
+        <v>256</v>
       </c>
       <c r="Q81" s="29"/>
       <c r="R81" s="29" t="s">
@@ -6925,7 +6943,7 @@
         <v>1.0</v>
       </c>
       <c r="B82" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
       <c r="C82">
         <v>3.0</v>
@@ -6953,13 +6971,13 @@
         <v>43</v>
       </c>
       <c r="L82" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="O82" s="21" t="s">
-        <v>253</v>
+        <v>259</v>
       </c>
       <c r="P82" s="21" t="s">
-        <v>253</v>
+        <v>259</v>
       </c>
       <c r="R82" t="s">
         <v>35</v>
@@ -6988,7 +7006,7 @@
         <v>1.0</v>
       </c>
       <c r="B83" t="s">
-        <v>254</v>
+        <v>260</v>
       </c>
       <c r="C83">
         <v>3.0</v>
@@ -7016,13 +7034,13 @@
         <v>43</v>
       </c>
       <c r="L83" t="s">
-        <v>255</v>
+        <v>261</v>
       </c>
       <c r="O83" s="21" t="s">
-        <v>256</v>
+        <v>262</v>
       </c>
       <c r="P83" s="21" t="s">
-        <v>256</v>
+        <v>262</v>
       </c>
       <c r="R83" t="s">
         <v>35</v>
@@ -7051,7 +7069,7 @@
         <v>1.0</v>
       </c>
       <c r="B84" t="s">
-        <v>257</v>
+        <v>263</v>
       </c>
       <c r="C84">
         <v>3.0</v>
@@ -7079,13 +7097,13 @@
         <v>43</v>
       </c>
       <c r="L84" t="s">
-        <v>258</v>
+        <v>264</v>
       </c>
       <c r="O84" s="21" t="s">
-        <v>259</v>
+        <v>265</v>
       </c>
       <c r="P84" s="21" t="s">
-        <v>259</v>
+        <v>265</v>
       </c>
       <c r="R84" t="s">
         <v>35</v>
@@ -7114,7 +7132,7 @@
         <v>1.0</v>
       </c>
       <c r="B85" s="29" t="s">
-        <v>260</v>
+        <v>266</v>
       </c>
       <c r="C85" s="29">
         <v>2.0</v>
@@ -7135,10 +7153,10 @@
       <c r="M85" s="29"/>
       <c r="N85" s="29"/>
       <c r="O85" s="31" t="s">
-        <v>261</v>
+        <v>267</v>
       </c>
       <c r="P85" s="31" t="s">
-        <v>261</v>
+        <v>267</v>
       </c>
       <c r="Q85" s="29"/>
       <c r="R85" s="29" t="s">
@@ -7170,7 +7188,7 @@
         <v>1.0</v>
       </c>
       <c r="B86" t="s">
-        <v>262</v>
+        <v>268</v>
       </c>
       <c r="C86">
         <v>3.0</v>
@@ -7198,13 +7216,13 @@
         <v>43</v>
       </c>
       <c r="L86" t="s">
-        <v>263</v>
+        <v>269</v>
       </c>
       <c r="O86" s="21" t="s">
-        <v>264</v>
+        <v>270</v>
       </c>
       <c r="P86" s="21" t="s">
-        <v>264</v>
+        <v>270</v>
       </c>
       <c r="R86" t="s">
         <v>35</v>
@@ -7233,7 +7251,7 @@
         <v>1.0</v>
       </c>
       <c r="B87" t="s">
-        <v>265</v>
+        <v>271</v>
       </c>
       <c r="C87">
         <v>3.0</v>
@@ -7261,13 +7279,13 @@
         <v>43</v>
       </c>
       <c r="L87" t="s">
-        <v>266</v>
+        <v>272</v>
       </c>
       <c r="O87" s="21" t="s">
-        <v>267</v>
+        <v>273</v>
       </c>
       <c r="P87" s="21" t="s">
-        <v>267</v>
+        <v>273</v>
       </c>
       <c r="R87" t="s">
         <v>35</v>
@@ -7296,7 +7314,7 @@
         <v>1.0</v>
       </c>
       <c r="B88" t="s">
-        <v>268</v>
+        <v>274</v>
       </c>
       <c r="C88">
         <v>3.0</v>
@@ -7324,13 +7342,13 @@
         <v>43</v>
       </c>
       <c r="L88" t="s">
-        <v>269</v>
+        <v>275</v>
       </c>
       <c r="O88" s="21" t="s">
-        <v>270</v>
+        <v>276</v>
       </c>
       <c r="P88" s="21" t="s">
-        <v>270</v>
+        <v>276</v>
       </c>
       <c r="R88" t="s">
         <v>35</v>
@@ -7359,7 +7377,7 @@
         <v>1.0</v>
       </c>
       <c r="B89" t="s">
-        <v>271</v>
+        <v>277</v>
       </c>
       <c r="C89">
         <v>3.0</v>
@@ -7387,13 +7405,13 @@
         <v>43</v>
       </c>
       <c r="L89" t="s">
-        <v>272</v>
+        <v>278</v>
       </c>
       <c r="O89" s="21" t="s">
-        <v>273</v>
+        <v>279</v>
       </c>
       <c r="P89" s="21" t="s">
-        <v>273</v>
+        <v>279</v>
       </c>
       <c r="R89" t="s">
         <v>35</v>
@@ -7422,7 +7440,7 @@
         <v>1.0</v>
       </c>
       <c r="B90" t="s">
-        <v>274</v>
+        <v>280</v>
       </c>
       <c r="C90">
         <v>3.0</v>
@@ -7450,13 +7468,13 @@
         <v>43</v>
       </c>
       <c r="L90" t="s">
-        <v>275</v>
+        <v>281</v>
       </c>
       <c r="O90" s="21" t="s">
-        <v>276</v>
+        <v>282</v>
       </c>
       <c r="P90" s="21" t="s">
-        <v>276</v>
+        <v>282</v>
       </c>
       <c r="R90" t="s">
         <v>35</v>
@@ -7485,7 +7503,7 @@
         <v>1.0</v>
       </c>
       <c r="B91" t="s">
-        <v>277</v>
+        <v>283</v>
       </c>
       <c r="C91">
         <v>3.0</v>
@@ -7513,13 +7531,13 @@
         <v>43</v>
       </c>
       <c r="L91" t="s">
-        <v>278</v>
+        <v>284</v>
       </c>
       <c r="O91" s="21" t="s">
-        <v>279</v>
+        <v>285</v>
       </c>
       <c r="P91" s="21" t="s">
-        <v>279</v>
+        <v>285</v>
       </c>
       <c r="R91" t="s">
         <v>35</v>
@@ -7548,7 +7566,7 @@
         <v>1.0</v>
       </c>
       <c r="B92" t="s">
-        <v>280</v>
+        <v>286</v>
       </c>
       <c r="C92">
         <v>3.0</v>
@@ -7576,13 +7594,13 @@
         <v>43</v>
       </c>
       <c r="L92" t="s">
-        <v>281</v>
+        <v>287</v>
       </c>
       <c r="O92" s="21" t="s">
-        <v>282</v>
+        <v>288</v>
       </c>
       <c r="P92" s="21" t="s">
-        <v>282</v>
+        <v>288</v>
       </c>
       <c r="R92" t="s">
         <v>35</v>
@@ -7612,7 +7630,7 @@
         <v>1.0</v>
       </c>
       <c r="B93" s="29" t="s">
-        <v>283</v>
+        <v>289</v>
       </c>
       <c r="C93" s="29">
         <v>2.0</v>
@@ -7633,10 +7651,10 @@
       <c r="M93" s="29"/>
       <c r="N93" s="29"/>
       <c r="O93" s="31" t="s">
-        <v>284</v>
+        <v>290</v>
       </c>
       <c r="P93" s="31" t="s">
-        <v>284</v>
+        <v>290</v>
       </c>
       <c r="Q93" s="29"/>
       <c r="R93" s="29" t="s">
@@ -7668,7 +7686,7 @@
         <v>1.0</v>
       </c>
       <c r="B94" t="s">
-        <v>285</v>
+        <v>291</v>
       </c>
       <c r="C94">
         <v>3.0</v>
@@ -7696,13 +7714,13 @@
         <v>43</v>
       </c>
       <c r="L94" t="s">
-        <v>286</v>
+        <v>292</v>
       </c>
       <c r="O94" s="21" t="s">
-        <v>287</v>
+        <v>293</v>
       </c>
       <c r="P94" s="21" t="s">
-        <v>287</v>
+        <v>293</v>
       </c>
       <c r="R94" t="s">
         <v>35</v>
@@ -7731,7 +7749,7 @@
         <v>1.0</v>
       </c>
       <c r="B95" t="s">
-        <v>288</v>
+        <v>294</v>
       </c>
       <c r="C95">
         <v>3.0</v>
@@ -7759,13 +7777,13 @@
         <v>43</v>
       </c>
       <c r="L95" t="s">
-        <v>289</v>
+        <v>295</v>
       </c>
       <c r="O95" s="21" t="s">
-        <v>290</v>
+        <v>296</v>
       </c>
       <c r="P95" s="21" t="s">
-        <v>290</v>
+        <v>296</v>
       </c>
       <c r="R95" t="s">
         <v>35</v>
@@ -7794,7 +7812,7 @@
         <v>1.0</v>
       </c>
       <c r="B96" s="29" t="s">
-        <v>291</v>
+        <v>297</v>
       </c>
       <c r="C96" s="29">
         <v>2.0</v>
@@ -7822,15 +7840,15 @@
         <v>43</v>
       </c>
       <c r="L96" s="29" t="s">
-        <v>292</v>
+        <v>298</v>
       </c>
       <c r="M96" s="29"/>
       <c r="N96" s="29"/>
       <c r="O96" s="31" t="s">
-        <v>293</v>
+        <v>299</v>
       </c>
       <c r="P96" s="31" t="s">
-        <v>293</v>
+        <v>299</v>
       </c>
       <c r="Q96" s="29"/>
       <c r="R96" s="29" t="s">
@@ -7870,7 +7888,7 @@
         <v>1.0</v>
       </c>
       <c r="B97" s="13" t="s">
-        <v>294</v>
+        <v>300</v>
       </c>
       <c r="C97" s="13">
         <v>1.0</v>
@@ -7891,10 +7909,10 @@
       <c r="M97" s="15"/>
       <c r="N97" s="15"/>
       <c r="O97" s="16" t="s">
-        <v>295</v>
+        <v>301</v>
       </c>
       <c r="P97" s="16" t="s">
-        <v>295</v>
+        <v>301</v>
       </c>
       <c r="Q97" s="15"/>
       <c r="R97" s="15" t="s">
@@ -7926,7 +7944,7 @@
         <v>1.0</v>
       </c>
       <c r="B98" s="29" t="s">
-        <v>296</v>
+        <v>302</v>
       </c>
       <c r="C98" s="29">
         <v>2.0</v>
@@ -7954,15 +7972,15 @@
         <v>43</v>
       </c>
       <c r="L98" s="29" t="s">
-        <v>297</v>
+        <v>303</v>
       </c>
       <c r="M98" s="29"/>
       <c r="N98" s="29"/>
       <c r="O98" s="31" t="s">
-        <v>298</v>
+        <v>304</v>
       </c>
       <c r="P98" s="31" t="s">
-        <v>298</v>
+        <v>304</v>
       </c>
       <c r="Q98" s="29"/>
       <c r="R98" s="29" t="s">
@@ -8004,7 +8022,7 @@
         <v>1.0</v>
       </c>
       <c r="B99" s="29" t="s">
-        <v>299</v>
+        <v>305</v>
       </c>
       <c r="C99" s="29">
         <v>2.0</v>
@@ -8032,15 +8050,15 @@
         <v>43</v>
       </c>
       <c r="L99" s="29" t="s">
-        <v>300</v>
+        <v>306</v>
       </c>
       <c r="M99" s="29"/>
       <c r="N99" s="29"/>
       <c r="O99" s="31" t="s">
-        <v>301</v>
+        <v>307</v>
       </c>
       <c r="P99" s="31" t="s">
-        <v>301</v>
+        <v>307</v>
       </c>
       <c r="Q99" s="29"/>
       <c r="R99" s="29" t="s">
@@ -8080,7 +8098,7 @@
         <v>1.0</v>
       </c>
       <c r="B100" s="29" t="s">
-        <v>302</v>
+        <v>308</v>
       </c>
       <c r="C100" s="29">
         <v>2.0</v>
@@ -8108,15 +8126,15 @@
         <v>43</v>
       </c>
       <c r="L100" s="29" t="s">
-        <v>303</v>
+        <v>309</v>
       </c>
       <c r="M100" s="29"/>
       <c r="N100" s="29"/>
       <c r="O100" s="31" t="s">
-        <v>304</v>
+        <v>310</v>
       </c>
       <c r="P100" s="31" t="s">
-        <v>304</v>
+        <v>310</v>
       </c>
       <c r="Q100" s="29"/>
       <c r="R100" s="29" t="s">
@@ -8156,7 +8174,7 @@
         <v>1.0</v>
       </c>
       <c r="B101" s="29" t="s">
-        <v>305</v>
+        <v>311</v>
       </c>
       <c r="C101" s="29">
         <v>2.0</v>
@@ -8184,15 +8202,15 @@
         <v>43</v>
       </c>
       <c r="L101" s="29" t="s">
-        <v>306</v>
+        <v>312</v>
       </c>
       <c r="M101" s="29"/>
       <c r="N101" s="29"/>
       <c r="O101" s="31" t="s">
-        <v>307</v>
+        <v>313</v>
       </c>
       <c r="P101" s="31" t="s">
-        <v>307</v>
+        <v>313</v>
       </c>
       <c r="Q101" s="29"/>
       <c r="R101" s="29" t="s">
@@ -8232,7 +8250,7 @@
         <v>1.0</v>
       </c>
       <c r="B102" s="29" t="s">
-        <v>308</v>
+        <v>314</v>
       </c>
       <c r="C102" s="29">
         <v>2.0</v>
@@ -8260,15 +8278,15 @@
         <v>43</v>
       </c>
       <c r="L102" s="29" t="s">
-        <v>309</v>
+        <v>315</v>
       </c>
       <c r="M102" s="29"/>
       <c r="N102" s="29"/>
       <c r="O102" s="31" t="s">
-        <v>310</v>
+        <v>316</v>
       </c>
       <c r="P102" s="31" t="s">
-        <v>310</v>
+        <v>316</v>
       </c>
       <c r="Q102" s="29"/>
       <c r="R102" s="29" t="s">
@@ -8309,7 +8327,7 @@
         <v>1.0</v>
       </c>
       <c r="B103" s="29" t="s">
-        <v>311</v>
+        <v>317</v>
       </c>
       <c r="C103" s="29">
         <v>2.0</v>
@@ -8337,15 +8355,15 @@
         <v>43</v>
       </c>
       <c r="L103" s="29" t="s">
-        <v>312</v>
+        <v>318</v>
       </c>
       <c r="M103" s="29"/>
       <c r="N103" s="29"/>
       <c r="O103" s="31" t="s">
-        <v>313</v>
+        <v>319</v>
       </c>
       <c r="P103" s="31" t="s">
-        <v>313</v>
+        <v>319</v>
       </c>
       <c r="Q103" s="29"/>
       <c r="R103" s="29" t="s">
@@ -8407,10 +8425,10 @@
       <c r="M104" s="29"/>
       <c r="N104" s="29"/>
       <c r="O104" s="31" t="s">
-        <v>314</v>
+        <v>320</v>
       </c>
       <c r="P104" s="31" t="s">
-        <v>314</v>
+        <v>320</v>
       </c>
       <c r="Q104" s="29"/>
       <c r="R104" s="29" t="s">
@@ -8442,7 +8460,7 @@
         <v>1.0</v>
       </c>
       <c r="B105" t="s">
-        <v>315</v>
+        <v>321</v>
       </c>
       <c r="C105">
         <v>3.0</v>
@@ -8470,13 +8488,13 @@
         <v>43</v>
       </c>
       <c r="L105" t="s">
-        <v>316</v>
+        <v>322</v>
       </c>
       <c r="O105" s="21" t="s">
-        <v>317</v>
+        <v>323</v>
       </c>
       <c r="P105" s="21" t="s">
-        <v>317</v>
+        <v>323</v>
       </c>
       <c r="R105" t="s">
         <v>35</v>
@@ -8507,7 +8525,7 @@
         <v>1.0</v>
       </c>
       <c r="B106" t="s">
-        <v>318</v>
+        <v>324</v>
       </c>
       <c r="C106">
         <v>3.0</v>
@@ -8535,13 +8553,13 @@
         <v>43</v>
       </c>
       <c r="L106" t="s">
-        <v>319</v>
+        <v>325</v>
       </c>
       <c r="O106" s="21" t="s">
-        <v>320</v>
+        <v>326</v>
       </c>
       <c r="P106" s="21" t="s">
-        <v>320</v>
+        <v>326</v>
       </c>
       <c r="R106" t="s">
         <v>35</v>
@@ -8572,7 +8590,7 @@
         <v>1.0</v>
       </c>
       <c r="B107" t="s">
-        <v>321</v>
+        <v>327</v>
       </c>
       <c r="C107">
         <v>3.0</v>
@@ -8600,13 +8618,13 @@
         <v>43</v>
       </c>
       <c r="L107" t="s">
-        <v>322</v>
+        <v>328</v>
       </c>
       <c r="O107" s="21" t="s">
-        <v>323</v>
+        <v>329</v>
       </c>
       <c r="P107" s="21" t="s">
-        <v>323</v>
+        <v>329</v>
       </c>
       <c r="R107" t="s">
         <v>35</v>
@@ -8637,7 +8655,7 @@
         <v>1.0</v>
       </c>
       <c r="B108" t="s">
-        <v>324</v>
+        <v>330</v>
       </c>
       <c r="C108">
         <v>3.0</v>
@@ -8665,13 +8683,13 @@
         <v>43</v>
       </c>
       <c r="L108" t="s">
-        <v>325</v>
+        <v>331</v>
       </c>
       <c r="O108" s="21" t="s">
-        <v>326</v>
+        <v>332</v>
       </c>
       <c r="P108" s="21" t="s">
-        <v>326</v>
+        <v>332</v>
       </c>
       <c r="R108" t="s">
         <v>35</v>
@@ -8702,7 +8720,7 @@
         <v>1.0</v>
       </c>
       <c r="B109" t="s">
-        <v>327</v>
+        <v>333</v>
       </c>
       <c r="C109">
         <v>3.0</v>
@@ -8730,13 +8748,13 @@
         <v>43</v>
       </c>
       <c r="L109" t="s">
-        <v>328</v>
+        <v>334</v>
       </c>
       <c r="O109" s="21" t="s">
-        <v>329</v>
+        <v>335</v>
       </c>
       <c r="P109" s="21" t="s">
-        <v>329</v>
+        <v>335</v>
       </c>
       <c r="R109" t="s">
         <v>35</v>
@@ -8767,7 +8785,7 @@
         <v>1.0</v>
       </c>
       <c r="B110" t="s">
-        <v>330</v>
+        <v>336</v>
       </c>
       <c r="C110">
         <v>3.0</v>
@@ -8795,13 +8813,13 @@
         <v>43</v>
       </c>
       <c r="L110" t="s">
-        <v>331</v>
+        <v>337</v>
       </c>
       <c r="O110" s="21" t="s">
-        <v>332</v>
+        <v>338</v>
       </c>
       <c r="P110" s="21" t="s">
-        <v>332</v>
+        <v>338</v>
       </c>
       <c r="R110" t="s">
         <v>35</v>
@@ -8832,7 +8850,7 @@
         <v>1.0</v>
       </c>
       <c r="B111" s="29" t="s">
-        <v>249</v>
+        <v>255</v>
       </c>
       <c r="C111" s="29">
         <v>2.0</v>
@@ -8853,10 +8871,10 @@
       <c r="M111" s="29"/>
       <c r="N111" s="29"/>
       <c r="O111" s="31" t="s">
-        <v>333</v>
+        <v>339</v>
       </c>
       <c r="P111" s="31" t="s">
-        <v>333</v>
+        <v>339</v>
       </c>
       <c r="Q111" s="29"/>
       <c r="R111" s="29" t="s">
@@ -8888,7 +8906,7 @@
         <v>1.0</v>
       </c>
       <c r="B112" t="s">
-        <v>334</v>
+        <v>340</v>
       </c>
       <c r="C112">
         <v>3.0</v>
@@ -8916,13 +8934,13 @@
         <v>43</v>
       </c>
       <c r="L112" t="s">
-        <v>335</v>
+        <v>341</v>
       </c>
       <c r="O112" s="21" t="s">
-        <v>336</v>
+        <v>342</v>
       </c>
       <c r="P112" s="21" t="s">
-        <v>336</v>
+        <v>342</v>
       </c>
       <c r="R112" t="s">
         <v>35</v>
@@ -8952,7 +8970,7 @@
         <v>1.0</v>
       </c>
       <c r="B113" t="s">
-        <v>337</v>
+        <v>343</v>
       </c>
       <c r="C113">
         <v>3.0</v>
@@ -8980,13 +8998,13 @@
         <v>43</v>
       </c>
       <c r="L113" t="s">
-        <v>338</v>
+        <v>344</v>
       </c>
       <c r="O113" s="21" t="s">
-        <v>339</v>
+        <v>345</v>
       </c>
       <c r="P113" s="21" t="s">
-        <v>339</v>
+        <v>345</v>
       </c>
       <c r="R113" t="s">
         <v>35</v>
@@ -9016,7 +9034,7 @@
         <v>1.0</v>
       </c>
       <c r="B114" t="s">
-        <v>340</v>
+        <v>346</v>
       </c>
       <c r="C114">
         <v>3.0</v>
@@ -9044,13 +9062,13 @@
         <v>43</v>
       </c>
       <c r="L114" t="s">
-        <v>341</v>
+        <v>347</v>
       </c>
       <c r="O114" s="21" t="s">
-        <v>342</v>
+        <v>348</v>
       </c>
       <c r="P114" s="21" t="s">
-        <v>342</v>
+        <v>348</v>
       </c>
       <c r="R114" t="s">
         <v>35</v>
@@ -9081,7 +9099,7 @@
         <v>1.0</v>
       </c>
       <c r="B115" t="s">
-        <v>343</v>
+        <v>349</v>
       </c>
       <c r="C115">
         <v>3.0</v>
@@ -9109,13 +9127,13 @@
         <v>43</v>
       </c>
       <c r="L115" t="s">
-        <v>344</v>
+        <v>350</v>
       </c>
       <c r="O115" s="21" t="s">
-        <v>345</v>
+        <v>351</v>
       </c>
       <c r="P115" s="21" t="s">
-        <v>345</v>
+        <v>351</v>
       </c>
       <c r="R115" t="s">
         <v>35</v>
@@ -9146,7 +9164,7 @@
         <v>1.0</v>
       </c>
       <c r="B116" t="s">
-        <v>346</v>
+        <v>352</v>
       </c>
       <c r="C116">
         <v>3.0</v>
@@ -9174,13 +9192,13 @@
         <v>43</v>
       </c>
       <c r="L116" t="s">
-        <v>347</v>
+        <v>353</v>
       </c>
       <c r="O116" s="21" t="s">
-        <v>348</v>
+        <v>354</v>
       </c>
       <c r="P116" s="21" t="s">
-        <v>348</v>
+        <v>354</v>
       </c>
       <c r="R116" t="s">
         <v>35</v>
@@ -9211,7 +9229,7 @@
         <v>1.0</v>
       </c>
       <c r="B117" t="s">
-        <v>349</v>
+        <v>355</v>
       </c>
       <c r="C117">
         <v>3.0</v>
@@ -9239,13 +9257,13 @@
         <v>43</v>
       </c>
       <c r="L117" t="s">
-        <v>350</v>
+        <v>356</v>
       </c>
       <c r="O117" s="21" t="s">
-        <v>351</v>
+        <v>357</v>
       </c>
       <c r="P117" s="21" t="s">
-        <v>351</v>
+        <v>357</v>
       </c>
       <c r="R117" t="s">
         <v>35</v>
@@ -9274,7 +9292,7 @@
         <v>1.0</v>
       </c>
       <c r="B118" s="29" t="s">
-        <v>352</v>
+        <v>358</v>
       </c>
       <c r="C118" s="29">
         <v>2.0</v>
@@ -9295,10 +9313,10 @@
       <c r="M118" s="29"/>
       <c r="N118" s="29"/>
       <c r="O118" s="31" t="s">
-        <v>353</v>
+        <v>359</v>
       </c>
       <c r="P118" s="31" t="s">
-        <v>353</v>
+        <v>359</v>
       </c>
       <c r="Q118" s="29"/>
       <c r="R118" s="29" t="s">
@@ -9330,7 +9348,7 @@
         <v>1.0</v>
       </c>
       <c r="B119" t="s">
-        <v>354</v>
+        <v>360</v>
       </c>
       <c r="C119">
         <v>3.0</v>
@@ -9358,13 +9376,13 @@
         <v>43</v>
       </c>
       <c r="L119" t="s">
-        <v>355</v>
+        <v>361</v>
       </c>
       <c r="O119" s="21" t="s">
-        <v>356</v>
+        <v>362</v>
       </c>
       <c r="P119" s="21" t="s">
-        <v>356</v>
+        <v>362</v>
       </c>
       <c r="R119" t="s">
         <v>35</v>
@@ -9394,7 +9412,7 @@
         <v>1.0</v>
       </c>
       <c r="B120" t="s">
-        <v>357</v>
+        <v>363</v>
       </c>
       <c r="C120">
         <v>3.0</v>
@@ -9422,13 +9440,13 @@
         <v>43</v>
       </c>
       <c r="L120" t="s">
-        <v>358</v>
+        <v>364</v>
       </c>
       <c r="O120" s="21" t="s">
-        <v>359</v>
+        <v>365</v>
       </c>
       <c r="P120" s="21" t="s">
-        <v>359</v>
+        <v>365</v>
       </c>
       <c r="R120" t="s">
         <v>35</v>
@@ -9458,7 +9476,7 @@
         <v>1.0</v>
       </c>
       <c r="B121" t="s">
-        <v>360</v>
+        <v>366</v>
       </c>
       <c r="C121">
         <v>3.0</v>
@@ -9486,13 +9504,13 @@
         <v>43</v>
       </c>
       <c r="L121" t="s">
-        <v>361</v>
+        <v>367</v>
       </c>
       <c r="O121" s="21" t="s">
-        <v>362</v>
+        <v>368</v>
       </c>
       <c r="P121" s="21" t="s">
-        <v>362</v>
+        <v>368</v>
       </c>
       <c r="R121" t="s">
         <v>35</v>
@@ -9522,7 +9540,7 @@
         <v>1.0</v>
       </c>
       <c r="B122" t="s">
-        <v>363</v>
+        <v>369</v>
       </c>
       <c r="C122">
         <v>3.0</v>
@@ -9550,13 +9568,13 @@
         <v>43</v>
       </c>
       <c r="L122" t="s">
-        <v>364</v>
+        <v>370</v>
       </c>
       <c r="O122" s="21" t="s">
-        <v>365</v>
+        <v>371</v>
       </c>
       <c r="P122" s="21" t="s">
-        <v>365</v>
+        <v>371</v>
       </c>
       <c r="R122" t="s">
         <v>35</v>
@@ -9586,7 +9604,7 @@
         <v>1.0</v>
       </c>
       <c r="B123" t="s">
-        <v>366</v>
+        <v>372</v>
       </c>
       <c r="C123">
         <v>3.0</v>
@@ -9614,13 +9632,13 @@
         <v>43</v>
       </c>
       <c r="L123" t="s">
-        <v>367</v>
+        <v>373</v>
       </c>
       <c r="O123" s="21" t="s">
-        <v>368</v>
+        <v>374</v>
       </c>
       <c r="P123" s="21" t="s">
-        <v>368</v>
+        <v>374</v>
       </c>
       <c r="R123" t="s">
         <v>35</v>
@@ -9650,7 +9668,7 @@
         <v>1.0</v>
       </c>
       <c r="B124" s="29" t="s">
-        <v>369</v>
+        <v>375</v>
       </c>
       <c r="C124" s="29">
         <v>2.0</v>
@@ -9671,10 +9689,10 @@
       <c r="M124" s="29"/>
       <c r="N124" s="29"/>
       <c r="O124" s="31" t="s">
-        <v>370</v>
+        <v>376</v>
       </c>
       <c r="P124" s="31" t="s">
-        <v>370</v>
+        <v>376</v>
       </c>
       <c r="Q124" s="29"/>
       <c r="R124" s="29" t="s">
@@ -9706,7 +9724,7 @@
         <v>1.0</v>
       </c>
       <c r="B125" t="s">
-        <v>371</v>
+        <v>377</v>
       </c>
       <c r="C125">
         <v>3.0</v>
@@ -9734,13 +9752,13 @@
         <v>43</v>
       </c>
       <c r="L125" t="s">
-        <v>372</v>
+        <v>378</v>
       </c>
       <c r="O125" s="21" t="s">
-        <v>373</v>
+        <v>379</v>
       </c>
       <c r="P125" s="21" t="s">
-        <v>373</v>
+        <v>379</v>
       </c>
       <c r="R125" t="s">
         <v>35</v>
@@ -9769,7 +9787,7 @@
         <v>1.0</v>
       </c>
       <c r="B126" s="29" t="s">
-        <v>374</v>
+        <v>380</v>
       </c>
       <c r="C126" s="29">
         <v>2.0</v>
@@ -9790,10 +9808,10 @@
       <c r="M126" s="29"/>
       <c r="N126" s="29"/>
       <c r="O126" s="31" t="s">
-        <v>375</v>
+        <v>381</v>
       </c>
       <c r="P126" s="31" t="s">
-        <v>375</v>
+        <v>381</v>
       </c>
       <c r="Q126" s="29"/>
       <c r="R126" s="29" t="s">
@@ -9825,7 +9843,7 @@
         <v>1.0</v>
       </c>
       <c r="B127" t="s">
-        <v>376</v>
+        <v>382</v>
       </c>
       <c r="C127">
         <v>3.0</v>
@@ -9853,13 +9871,13 @@
         <v>43</v>
       </c>
       <c r="L127" t="s">
-        <v>377</v>
+        <v>383</v>
       </c>
       <c r="O127" s="21" t="s">
-        <v>378</v>
+        <v>384</v>
       </c>
       <c r="P127" s="21" t="s">
-        <v>378</v>
+        <v>384</v>
       </c>
       <c r="R127" t="s">
         <v>35</v>
@@ -9888,7 +9906,7 @@
         <v>1.0</v>
       </c>
       <c r="B128" t="s">
-        <v>379</v>
+        <v>385</v>
       </c>
       <c r="C128">
         <v>3.0</v>
@@ -9916,13 +9934,13 @@
         <v>43</v>
       </c>
       <c r="L128" t="s">
-        <v>380</v>
+        <v>386</v>
       </c>
       <c r="O128" s="21" t="s">
-        <v>381</v>
+        <v>387</v>
       </c>
       <c r="P128" s="21" t="s">
-        <v>381</v>
+        <v>387</v>
       </c>
       <c r="R128" t="s">
         <v>35</v>
@@ -9951,7 +9969,7 @@
         <v>1.0</v>
       </c>
       <c r="B129" s="13" t="s">
-        <v>382</v>
+        <v>388</v>
       </c>
       <c r="C129" s="13">
         <v>1.0</v>
@@ -9979,15 +9997,15 @@
         <v>43</v>
       </c>
       <c r="L129" s="15" t="s">
-        <v>383</v>
+        <v>389</v>
       </c>
       <c r="M129" s="15"/>
       <c r="N129" s="15"/>
       <c r="O129" s="16" t="s">
-        <v>384</v>
+        <v>390</v>
       </c>
       <c r="P129" s="16" t="s">
-        <v>384</v>
+        <v>390</v>
       </c>
       <c r="Q129" s="15"/>
       <c r="R129" s="15" t="s">
@@ -10027,7 +10045,7 @@
         <v>1.0</v>
       </c>
       <c r="B130" s="13" t="s">
-        <v>385</v>
+        <v>391</v>
       </c>
       <c r="C130" s="13">
         <v>1.0</v>
@@ -10055,15 +10073,15 @@
         <v>43</v>
       </c>
       <c r="L130" s="15" t="s">
-        <v>386</v>
+        <v>392</v>
       </c>
       <c r="M130" s="15"/>
       <c r="N130" s="15"/>
       <c r="O130" s="16" t="s">
-        <v>387</v>
+        <v>393</v>
       </c>
       <c r="P130" s="16" t="s">
-        <v>387</v>
+        <v>393</v>
       </c>
       <c r="Q130" s="15"/>
       <c r="R130" s="15" t="s">
@@ -10103,7 +10121,7 @@
         <v>1.0</v>
       </c>
       <c r="B131" s="13" t="s">
-        <v>388</v>
+        <v>394</v>
       </c>
       <c r="C131" s="13">
         <v>1.0</v>
@@ -10131,15 +10149,15 @@
         <v>43</v>
       </c>
       <c r="L131" s="15" t="s">
-        <v>389</v>
+        <v>395</v>
       </c>
       <c r="M131" s="15"/>
       <c r="N131" s="15"/>
       <c r="O131" s="16" t="s">
-        <v>390</v>
+        <v>396</v>
       </c>
       <c r="P131" s="16" t="s">
-        <v>390</v>
+        <v>396</v>
       </c>
       <c r="Q131" s="15"/>
       <c r="R131" s="15" t="s">
@@ -10179,7 +10197,7 @@
         <v>1.0</v>
       </c>
       <c r="B132" s="13" t="s">
-        <v>391</v>
+        <v>397</v>
       </c>
       <c r="C132" s="13">
         <v>1.0</v>
@@ -10207,15 +10225,15 @@
         <v>43</v>
       </c>
       <c r="L132" s="15" t="s">
-        <v>392</v>
+        <v>398</v>
       </c>
       <c r="M132" s="15"/>
       <c r="N132" s="15"/>
       <c r="O132" s="16" t="s">
-        <v>393</v>
+        <v>399</v>
       </c>
       <c r="P132" s="16" t="s">
-        <v>393</v>
+        <v>399</v>
       </c>
       <c r="Q132" s="15"/>
       <c r="R132" s="15" t="s">
@@ -10255,7 +10273,7 @@
         <v>1.0</v>
       </c>
       <c r="B133" s="5" t="s">
-        <v>394</v>
+        <v>400</v>
       </c>
       <c r="C133" s="5">
         <v>0.0</v>
@@ -10311,7 +10329,7 @@
         <v>1.0</v>
       </c>
       <c r="B134" t="s">
-        <v>395</v>
+        <v>401</v>
       </c>
       <c r="C134">
         <v>1.0</v>
@@ -10339,13 +10357,13 @@
         <v>43</v>
       </c>
       <c r="L134" t="s">
-        <v>396</v>
+        <v>402</v>
       </c>
       <c r="O134" s="21" t="s">
-        <v>397</v>
+        <v>403</v>
       </c>
       <c r="P134" s="21" t="s">
-        <v>397</v>
+        <v>403</v>
       </c>
       <c r="R134" t="s">
         <v>35</v>
@@ -10374,7 +10392,7 @@
         <v>1.0</v>
       </c>
       <c r="B135" t="s">
-        <v>398</v>
+        <v>404</v>
       </c>
       <c r="C135">
         <v>1.0</v>
@@ -10402,13 +10420,13 @@
         <v>43</v>
       </c>
       <c r="L135" t="s">
-        <v>399</v>
+        <v>405</v>
       </c>
       <c r="O135" s="21" t="s">
-        <v>400</v>
+        <v>406</v>
       </c>
       <c r="P135" s="21" t="s">
-        <v>400</v>
+        <v>406</v>
       </c>
       <c r="R135" t="s">
         <v>35</v>
@@ -10437,7 +10455,7 @@
         <v>1.0</v>
       </c>
       <c r="B136" t="s">
-        <v>401</v>
+        <v>407</v>
       </c>
       <c r="C136">
         <v>1.0</v>
@@ -10465,13 +10483,13 @@
         <v>43</v>
       </c>
       <c r="L136" t="s">
-        <v>402</v>
+        <v>408</v>
       </c>
       <c r="O136" s="21" t="s">
-        <v>403</v>
+        <v>409</v>
       </c>
       <c r="P136" s="21" t="s">
-        <v>403</v>
+        <v>409</v>
       </c>
       <c r="R136" t="s">
         <v>35</v>
@@ -10500,7 +10518,7 @@
         <v>1.0</v>
       </c>
       <c r="B137" t="s">
-        <v>404</v>
+        <v>410</v>
       </c>
       <c r="C137">
         <v>1.0</v>
@@ -10528,13 +10546,13 @@
         <v>43</v>
       </c>
       <c r="L137" t="s">
-        <v>405</v>
+        <v>411</v>
       </c>
       <c r="O137" s="21" t="s">
-        <v>406</v>
+        <v>412</v>
       </c>
       <c r="P137" s="21" t="s">
-        <v>406</v>
+        <v>412</v>
       </c>
       <c r="R137" t="s">
         <v>35</v>
@@ -10563,7 +10581,7 @@
         <v>1.0</v>
       </c>
       <c r="B138" t="s">
-        <v>407</v>
+        <v>413</v>
       </c>
       <c r="C138">
         <v>1.0</v>
@@ -10591,13 +10609,13 @@
         <v>43</v>
       </c>
       <c r="L138" t="s">
-        <v>408</v>
+        <v>414</v>
       </c>
       <c r="O138" s="21" t="s">
-        <v>409</v>
+        <v>415</v>
       </c>
       <c r="P138" s="21" t="s">
-        <v>409</v>
+        <v>415</v>
       </c>
       <c r="R138" t="s">
         <v>35</v>
@@ -10626,7 +10644,7 @@
         <v>1.0</v>
       </c>
       <c r="B139" t="s">
-        <v>410</v>
+        <v>416</v>
       </c>
       <c r="C139">
         <v>1.0</v>
@@ -10654,13 +10672,13 @@
         <v>43</v>
       </c>
       <c r="L139" t="s">
-        <v>411</v>
+        <v>417</v>
       </c>
       <c r="O139" s="21" t="s">
-        <v>412</v>
+        <v>418</v>
       </c>
       <c r="P139" s="21" t="s">
-        <v>412</v>
+        <v>418</v>
       </c>
       <c r="R139" t="s">
         <v>35</v>
@@ -10689,7 +10707,7 @@
         <v>1.0</v>
       </c>
       <c r="B140" s="5" t="s">
-        <v>413</v>
+        <v>419</v>
       </c>
       <c r="C140" s="5">
         <v>0.0</v>
@@ -10745,7 +10763,7 @@
         <v>1.0</v>
       </c>
       <c r="B141" t="s">
-        <v>414</v>
+        <v>420</v>
       </c>
       <c r="C141">
         <v>1.0</v>
@@ -10773,13 +10791,13 @@
         <v>43</v>
       </c>
       <c r="L141" t="s">
-        <v>415</v>
+        <v>421</v>
       </c>
       <c r="O141" s="21" t="s">
-        <v>416</v>
+        <v>422</v>
       </c>
       <c r="P141" s="21" t="s">
-        <v>416</v>
+        <v>422</v>
       </c>
       <c r="R141" t="s">
         <v>35</v>
@@ -10808,7 +10826,7 @@
         <v>1.0</v>
       </c>
       <c r="B142" t="s">
-        <v>417</v>
+        <v>423</v>
       </c>
       <c r="C142">
         <v>1.0</v>
@@ -10836,13 +10854,13 @@
         <v>43</v>
       </c>
       <c r="L142" t="s">
-        <v>418</v>
+        <v>424</v>
       </c>
       <c r="O142" s="21" t="s">
-        <v>419</v>
+        <v>425</v>
       </c>
       <c r="P142" s="21" t="s">
-        <v>419</v>
+        <v>425</v>
       </c>
       <c r="R142" t="s">
         <v>35</v>
@@ -10871,7 +10889,7 @@
         <v>1.0</v>
       </c>
       <c r="B143" t="s">
-        <v>420</v>
+        <v>426</v>
       </c>
       <c r="C143">
         <v>1.0</v>
@@ -10899,13 +10917,13 @@
         <v>43</v>
       </c>
       <c r="L143" t="s">
-        <v>421</v>
+        <v>427</v>
       </c>
       <c r="O143" s="21" t="s">
-        <v>422</v>
+        <v>428</v>
       </c>
       <c r="P143" s="21" t="s">
-        <v>422</v>
+        <v>428</v>
       </c>
       <c r="R143" t="s">
         <v>35</v>
@@ -10935,7 +10953,7 @@
         <v>1.0</v>
       </c>
       <c r="B144" t="s">
-        <v>423</v>
+        <v>429</v>
       </c>
       <c r="C144">
         <v>1.0</v>
@@ -10963,13 +10981,13 @@
         <v>43</v>
       </c>
       <c r="L144" t="s">
-        <v>424</v>
+        <v>430</v>
       </c>
       <c r="O144" s="21" t="s">
-        <v>425</v>
+        <v>431</v>
       </c>
       <c r="P144" s="21" t="s">
-        <v>425</v>
+        <v>431</v>
       </c>
       <c r="R144" t="s">
         <v>35</v>
@@ -10998,7 +11016,7 @@
         <v>1.0</v>
       </c>
       <c r="B145" t="s">
-        <v>426</v>
+        <v>432</v>
       </c>
       <c r="C145">
         <v>1.0</v>
@@ -11026,13 +11044,13 @@
         <v>43</v>
       </c>
       <c r="L145" t="s">
-        <v>427</v>
+        <v>433</v>
       </c>
       <c r="O145" s="21" t="s">
-        <v>428</v>
+        <v>434</v>
       </c>
       <c r="P145" s="21" t="s">
-        <v>428</v>
+        <v>434</v>
       </c>
       <c r="R145" t="s">
         <v>35</v>
@@ -11062,7 +11080,7 @@
         <v>1.0</v>
       </c>
       <c r="B146" t="s">
-        <v>429</v>
+        <v>435</v>
       </c>
       <c r="C146">
         <v>1.0</v>
@@ -11090,13 +11108,13 @@
         <v>43</v>
       </c>
       <c r="L146" t="s">
-        <v>430</v>
+        <v>436</v>
       </c>
       <c r="O146" s="21" t="s">
-        <v>431</v>
+        <v>437</v>
       </c>
       <c r="P146" s="21" t="s">
-        <v>431</v>
+        <v>437</v>
       </c>
       <c r="R146" t="s">
         <v>35</v>
@@ -11125,7 +11143,7 @@
         <v>1.0</v>
       </c>
       <c r="B147" t="s">
-        <v>432</v>
+        <v>438</v>
       </c>
       <c r="C147">
         <v>1.0</v>
@@ -11153,13 +11171,13 @@
         <v>43</v>
       </c>
       <c r="L147" t="s">
-        <v>433</v>
+        <v>439</v>
       </c>
       <c r="O147" s="21" t="s">
-        <v>434</v>
+        <v>440</v>
       </c>
       <c r="P147" s="21" t="s">
-        <v>434</v>
+        <v>440</v>
       </c>
       <c r="R147" t="s">
         <v>35</v>
@@ -11188,7 +11206,7 @@
         <v>1.0</v>
       </c>
       <c r="B148" t="s">
-        <v>435</v>
+        <v>441</v>
       </c>
       <c r="C148">
         <v>1.0</v>
@@ -11216,13 +11234,13 @@
         <v>43</v>
       </c>
       <c r="L148" t="s">
-        <v>436</v>
+        <v>442</v>
       </c>
       <c r="O148" s="21" t="s">
-        <v>437</v>
+        <v>443</v>
       </c>
       <c r="P148" s="21" t="s">
-        <v>437</v>
+        <v>443</v>
       </c>
       <c r="R148" t="s">
         <v>35</v>
@@ -11251,7 +11269,7 @@
         <v>1.0</v>
       </c>
       <c r="B149" s="25" t="s">
-        <v>438</v>
+        <v>444</v>
       </c>
       <c r="C149">
         <v>1.0</v>
@@ -11279,13 +11297,13 @@
         <v>43</v>
       </c>
       <c r="L149" s="25" t="s">
-        <v>439</v>
+        <v>445</v>
       </c>
       <c r="O149" s="21" t="s">
-        <v>440</v>
+        <v>446</v>
       </c>
       <c r="P149" s="21" t="s">
-        <v>440</v>
+        <v>446</v>
       </c>
       <c r="R149" t="s">
         <v>35</v>
@@ -11314,7 +11332,7 @@
         <v>1.0</v>
       </c>
       <c r="B150" s="5" t="s">
-        <v>441</v>
+        <v>447</v>
       </c>
       <c r="C150" s="5">
         <v>0.0</v>
@@ -11370,7 +11388,7 @@
         <v>1.0</v>
       </c>
       <c r="B151" s="13" t="s">
-        <v>442</v>
+        <v>448</v>
       </c>
       <c r="C151" s="13">
         <v>1.0</v>
@@ -11391,10 +11409,10 @@
       <c r="M151" s="15"/>
       <c r="N151" s="15"/>
       <c r="O151" s="16" t="s">
-        <v>443</v>
+        <v>449</v>
       </c>
       <c r="P151" s="16" t="s">
-        <v>443</v>
+        <v>449</v>
       </c>
       <c r="Q151" s="15"/>
       <c r="R151" s="15" t="s">
@@ -11426,7 +11444,7 @@
         <v>1.0</v>
       </c>
       <c r="B152" t="s">
-        <v>444</v>
+        <v>450</v>
       </c>
       <c r="C152">
         <v>2.0</v>
@@ -11454,13 +11472,13 @@
         <v>43</v>
       </c>
       <c r="L152" t="s">
-        <v>445</v>
+        <v>451</v>
       </c>
       <c r="O152" s="21" t="s">
-        <v>446</v>
+        <v>452</v>
       </c>
       <c r="P152" s="21" t="s">
-        <v>446</v>
+        <v>452</v>
       </c>
       <c r="R152" t="s">
         <v>35</v>
@@ -11490,7 +11508,7 @@
         <v>1.0</v>
       </c>
       <c r="B153" t="s">
-        <v>447</v>
+        <v>453</v>
       </c>
       <c r="C153">
         <v>2.0</v>
@@ -11518,13 +11536,13 @@
         <v>43</v>
       </c>
       <c r="L153" t="s">
-        <v>448</v>
+        <v>454</v>
       </c>
       <c r="O153" s="21" t="s">
-        <v>449</v>
+        <v>455</v>
       </c>
       <c r="P153" s="21" t="s">
-        <v>449</v>
+        <v>455</v>
       </c>
       <c r="R153" t="s">
         <v>35</v>
@@ -11554,7 +11572,7 @@
         <v>1.0</v>
       </c>
       <c r="B154" t="s">
-        <v>450</v>
+        <v>456</v>
       </c>
       <c r="C154">
         <v>2.0</v>
@@ -11582,13 +11600,13 @@
         <v>43</v>
       </c>
       <c r="L154" t="s">
-        <v>451</v>
+        <v>457</v>
       </c>
       <c r="O154" s="21" t="s">
-        <v>452</v>
+        <v>458</v>
       </c>
       <c r="P154" s="21" t="s">
-        <v>452</v>
+        <v>458</v>
       </c>
       <c r="R154" t="s">
         <v>35</v>
@@ -11618,7 +11636,7 @@
         <v>1.0</v>
       </c>
       <c r="B155" t="s">
-        <v>453</v>
+        <v>459</v>
       </c>
       <c r="C155">
         <v>2.0</v>
@@ -11646,13 +11664,13 @@
         <v>43</v>
       </c>
       <c r="L155" t="s">
-        <v>454</v>
+        <v>460</v>
       </c>
       <c r="O155" s="21" t="s">
-        <v>455</v>
+        <v>461</v>
       </c>
       <c r="P155" s="21" t="s">
-        <v>455</v>
+        <v>461</v>
       </c>
       <c r="R155" t="s">
         <v>35</v>
@@ -11682,7 +11700,7 @@
         <v>1.0</v>
       </c>
       <c r="B156" t="s">
-        <v>456</v>
+        <v>462</v>
       </c>
       <c r="C156">
         <v>2.0</v>
@@ -11710,13 +11728,13 @@
         <v>43</v>
       </c>
       <c r="L156" t="s">
-        <v>457</v>
+        <v>463</v>
       </c>
       <c r="O156" s="21" t="s">
-        <v>458</v>
+        <v>464</v>
       </c>
       <c r="P156" s="21" t="s">
-        <v>458</v>
+        <v>464</v>
       </c>
       <c r="R156" t="s">
         <v>35</v>
@@ -11746,7 +11764,7 @@
         <v>1.0</v>
       </c>
       <c r="B157" s="13" t="s">
-        <v>459</v>
+        <v>465</v>
       </c>
       <c r="C157" s="13">
         <v>1.0</v>
@@ -11767,10 +11785,10 @@
       <c r="M157" s="15"/>
       <c r="N157" s="15"/>
       <c r="O157" s="16" t="s">
-        <v>460</v>
+        <v>466</v>
       </c>
       <c r="P157" s="16" t="s">
-        <v>460</v>
+        <v>466</v>
       </c>
       <c r="Q157" s="15"/>
       <c r="R157" s="15" t="s">
@@ -11802,7 +11820,7 @@
         <v>1.0</v>
       </c>
       <c r="B158" t="s">
-        <v>461</v>
+        <v>467</v>
       </c>
       <c r="C158">
         <v>2.0</v>
@@ -11830,13 +11848,13 @@
         <v>43</v>
       </c>
       <c r="L158" t="s">
-        <v>462</v>
+        <v>468</v>
       </c>
       <c r="O158" s="21" t="s">
-        <v>463</v>
+        <v>469</v>
       </c>
       <c r="P158" s="21" t="s">
-        <v>463</v>
+        <v>469</v>
       </c>
       <c r="R158" t="s">
         <v>35</v>
@@ -11866,7 +11884,7 @@
         <v>1.0</v>
       </c>
       <c r="B159" t="s">
-        <v>464</v>
+        <v>470</v>
       </c>
       <c r="C159">
         <v>2.0</v>
@@ -11894,13 +11912,13 @@
         <v>43</v>
       </c>
       <c r="L159" t="s">
-        <v>465</v>
+        <v>471</v>
       </c>
       <c r="O159" s="21" t="s">
-        <v>466</v>
+        <v>472</v>
       </c>
       <c r="P159" s="21" t="s">
-        <v>466</v>
+        <v>472</v>
       </c>
       <c r="R159" t="s">
         <v>35</v>
@@ -11930,7 +11948,7 @@
         <v>1.0</v>
       </c>
       <c r="B160" t="s">
-        <v>467</v>
+        <v>473</v>
       </c>
       <c r="C160">
         <v>2.0</v>
@@ -11958,13 +11976,13 @@
         <v>43</v>
       </c>
       <c r="L160" t="s">
-        <v>468</v>
+        <v>474</v>
       </c>
       <c r="O160" s="21" t="s">
-        <v>469</v>
+        <v>475</v>
       </c>
       <c r="P160" s="21" t="s">
-        <v>469</v>
+        <v>475</v>
       </c>
       <c r="R160" t="s">
         <v>35</v>
@@ -11994,7 +12012,7 @@
         <v>1.0</v>
       </c>
       <c r="B161" t="s">
-        <v>470</v>
+        <v>476</v>
       </c>
       <c r="C161">
         <v>2.0</v>
@@ -12022,13 +12040,13 @@
         <v>43</v>
       </c>
       <c r="L161" t="s">
-        <v>471</v>
+        <v>477</v>
       </c>
       <c r="O161" s="21" t="s">
-        <v>472</v>
+        <v>478</v>
       </c>
       <c r="P161" s="21" t="s">
-        <v>472</v>
+        <v>478</v>
       </c>
       <c r="R161" t="s">
         <v>35</v>
@@ -12058,7 +12076,7 @@
         <v>1.0</v>
       </c>
       <c r="B162" t="s">
-        <v>473</v>
+        <v>479</v>
       </c>
       <c r="C162">
         <v>2.0</v>
@@ -12086,13 +12104,13 @@
         <v>43</v>
       </c>
       <c r="L162" t="s">
-        <v>474</v>
+        <v>480</v>
       </c>
       <c r="O162" s="21" t="s">
-        <v>475</v>
+        <v>481</v>
       </c>
       <c r="P162" s="21" t="s">
-        <v>475</v>
+        <v>481</v>
       </c>
       <c r="R162" t="s">
         <v>35</v>
@@ -12122,7 +12140,7 @@
         <v>1.0</v>
       </c>
       <c r="B163" s="5" t="s">
-        <v>476</v>
+        <v>482</v>
       </c>
       <c r="C163" s="5">
         <v>0.0</v>
@@ -12178,7 +12196,7 @@
         <v>1.0</v>
       </c>
       <c r="B164" s="13" t="s">
-        <v>477</v>
+        <v>483</v>
       </c>
       <c r="C164" s="13">
         <v>1.0</v>
@@ -12199,10 +12217,10 @@
       <c r="M164" s="15"/>
       <c r="N164" s="15"/>
       <c r="O164" s="16" t="s">
-        <v>478</v>
+        <v>484</v>
       </c>
       <c r="P164" s="16" t="s">
-        <v>478</v>
+        <v>484</v>
       </c>
       <c r="Q164" s="15"/>
       <c r="R164" s="15" t="s">
@@ -12234,7 +12252,7 @@
         <v>1.0</v>
       </c>
       <c r="B165" t="s">
-        <v>479</v>
+        <v>485</v>
       </c>
       <c r="C165">
         <v>2.0</v>
@@ -12262,13 +12280,13 @@
         <v>43</v>
       </c>
       <c r="L165" t="s">
-        <v>480</v>
+        <v>486</v>
       </c>
       <c r="O165" s="21" t="s">
-        <v>481</v>
+        <v>487</v>
       </c>
       <c r="P165" s="21" t="s">
-        <v>481</v>
+        <v>487</v>
       </c>
       <c r="R165" t="s">
         <v>35</v>
@@ -12299,7 +12317,7 @@
         <v>1.0</v>
       </c>
       <c r="B166" t="s">
-        <v>482</v>
+        <v>488</v>
       </c>
       <c r="C166">
         <v>2.0</v>
@@ -12327,13 +12345,13 @@
         <v>43</v>
       </c>
       <c r="L166" t="s">
-        <v>483</v>
+        <v>489</v>
       </c>
       <c r="O166" s="21" t="s">
-        <v>484</v>
+        <v>490</v>
       </c>
       <c r="P166" s="21" t="s">
-        <v>484</v>
+        <v>490</v>
       </c>
       <c r="R166" t="s">
         <v>35</v>
@@ -12363,7 +12381,7 @@
         <v>1.0</v>
       </c>
       <c r="B167" t="s">
-        <v>485</v>
+        <v>491</v>
       </c>
       <c r="C167">
         <v>2.0</v>
@@ -12391,13 +12409,13 @@
         <v>43</v>
       </c>
       <c r="L167" t="s">
-        <v>486</v>
+        <v>492</v>
       </c>
       <c r="O167" s="21" t="s">
-        <v>487</v>
+        <v>493</v>
       </c>
       <c r="P167" s="21" t="s">
-        <v>487</v>
+        <v>493</v>
       </c>
       <c r="R167" t="s">
         <v>35</v>
@@ -12427,7 +12445,7 @@
         <v>1.0</v>
       </c>
       <c r="B168" t="s">
-        <v>488</v>
+        <v>494</v>
       </c>
       <c r="C168">
         <v>2.0</v>
@@ -12455,13 +12473,13 @@
         <v>43</v>
       </c>
       <c r="L168" t="s">
-        <v>489</v>
+        <v>495</v>
       </c>
       <c r="O168" s="21" t="s">
-        <v>490</v>
+        <v>496</v>
       </c>
       <c r="P168" s="21" t="s">
-        <v>490</v>
+        <v>496</v>
       </c>
       <c r="R168" t="s">
         <v>35</v>
@@ -12491,7 +12509,7 @@
         <v>1.0</v>
       </c>
       <c r="B169" t="s">
-        <v>491</v>
+        <v>497</v>
       </c>
       <c r="C169">
         <v>2.0</v>
@@ -12519,13 +12537,13 @@
         <v>43</v>
       </c>
       <c r="L169" t="s">
-        <v>492</v>
+        <v>498</v>
       </c>
       <c r="O169" s="21" t="s">
-        <v>493</v>
+        <v>499</v>
       </c>
       <c r="P169" s="21" t="s">
-        <v>493</v>
+        <v>499</v>
       </c>
       <c r="R169" t="s">
         <v>35</v>
@@ -12555,7 +12573,7 @@
         <v>1.0</v>
       </c>
       <c r="B170" s="13" t="s">
-        <v>494</v>
+        <v>500</v>
       </c>
       <c r="C170" s="13">
         <v>1.0</v>
@@ -12576,10 +12594,10 @@
       <c r="M170" s="15"/>
       <c r="N170" s="15"/>
       <c r="O170" s="16" t="s">
-        <v>495</v>
+        <v>501</v>
       </c>
       <c r="P170" s="16" t="s">
-        <v>495</v>
+        <v>501</v>
       </c>
       <c r="Q170" s="15"/>
       <c r="R170" s="15" t="s">
@@ -12611,7 +12629,7 @@
         <v>1.0</v>
       </c>
       <c r="B171" t="s">
-        <v>496</v>
+        <v>502</v>
       </c>
       <c r="C171">
         <v>2.0</v>
@@ -12639,13 +12657,13 @@
         <v>43</v>
       </c>
       <c r="L171" t="s">
-        <v>497</v>
+        <v>503</v>
       </c>
       <c r="O171" s="21" t="s">
-        <v>498</v>
+        <v>504</v>
       </c>
       <c r="P171" s="21" t="s">
-        <v>498</v>
+        <v>504</v>
       </c>
       <c r="R171" t="s">
         <v>35</v>
@@ -12675,7 +12693,7 @@
         <v>1.0</v>
       </c>
       <c r="B172" t="s">
-        <v>499</v>
+        <v>505</v>
       </c>
       <c r="C172">
         <v>2.0</v>
@@ -12703,13 +12721,13 @@
         <v>43</v>
       </c>
       <c r="L172" t="s">
-        <v>500</v>
+        <v>506</v>
       </c>
       <c r="O172" s="21" t="s">
-        <v>501</v>
+        <v>507</v>
       </c>
       <c r="P172" s="21" t="s">
-        <v>501</v>
+        <v>507</v>
       </c>
       <c r="R172" t="s">
         <v>35</v>
@@ -12739,7 +12757,7 @@
         <v>1.0</v>
       </c>
       <c r="B173" t="s">
-        <v>502</v>
+        <v>508</v>
       </c>
       <c r="C173">
         <v>2.0</v>
@@ -12767,13 +12785,13 @@
         <v>43</v>
       </c>
       <c r="L173" t="s">
-        <v>503</v>
+        <v>509</v>
       </c>
       <c r="O173" s="21" t="s">
-        <v>504</v>
+        <v>510</v>
       </c>
       <c r="P173" s="21" t="s">
-        <v>504</v>
+        <v>510</v>
       </c>
       <c r="R173" t="s">
         <v>35</v>
@@ -12803,7 +12821,7 @@
         <v>1.0</v>
       </c>
       <c r="B174" t="s">
-        <v>505</v>
+        <v>511</v>
       </c>
       <c r="C174">
         <v>2.0</v>
@@ -12831,13 +12849,13 @@
         <v>43</v>
       </c>
       <c r="L174" t="s">
-        <v>506</v>
+        <v>512</v>
       </c>
       <c r="O174" s="21" t="s">
-        <v>507</v>
+        <v>513</v>
       </c>
       <c r="P174" s="21" t="s">
-        <v>507</v>
+        <v>513</v>
       </c>
       <c r="R174" t="s">
         <v>35</v>

</xml_diff>